<commit_message>
refactor: Improve filter logic; remove V1 artifacts
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Customer</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>Included</t>
   </si>
   <si>
-    <t>Non-Billable</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -145,6 +139,9 @@
   </si>
   <si>
     <t>Redirects</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
@@ -636,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -649,304 +646,290 @@
     <col min="3" max="3" width="11.83203125" style="12" customWidth="1"/>
     <col min="4" max="4" width="3.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.1640625" style="12" customWidth="1"/>
-    <col min="8" max="9" width="6.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" style="12" customWidth="1"/>
+    <col min="7" max="8" width="6.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="34">
+    <row r="1" spans="1:10" ht="23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="17">
+        <v>26</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17">
       <c r="A2" s="6">
         <v>43101</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
-        <v>8</v>
+      <c r="G2" s="9">
+        <v>0.3611111111111111</v>
       </c>
       <c r="H2" s="9">
-        <v>0.3611111111111111</v>
+        <v>0.3923611111111111</v>
       </c>
       <c r="I2" s="9">
-        <v>0.3923611111111111</v>
-      </c>
-      <c r="J2" s="9">
-        <f>IF(AND(H2&lt;&gt;"",I2&lt;&gt;""),I2-H2,"")</f>
+        <f>IF(AND(G2&lt;&gt;"",H2&lt;&gt;""),H2-G2,"")</f>
         <v>3.125E-2</v>
       </c>
-      <c r="K2" s="10">
-        <f t="shared" ref="K2:K27" si="0">IF(J2&lt;&gt;"",J2*24,"")</f>
+      <c r="J2" s="10">
+        <f t="shared" ref="J2:J27" si="0">IF(I2&lt;&gt;"",I2*24,"")</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17">
+    <row r="3" spans="1:10" ht="17">
       <c r="A3" s="6">
         <v>43102</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="7" t="s">
-        <v>10</v>
+      <c r="G3" s="9">
+        <v>0.3125</v>
       </c>
       <c r="H3" s="9">
-        <v>0.3125</v>
+        <v>0.3215277777777778</v>
       </c>
       <c r="I3" s="9">
-        <v>0.3215277777777778</v>
-      </c>
-      <c r="J3" s="9">
-        <f>IF(AND(H3&lt;&gt;"",I3&lt;&gt;""),I3-H3,"")</f>
+        <f>IF(AND(G3&lt;&gt;"",H3&lt;&gt;""),H3-G3,"")</f>
         <v>9.0277777777778012E-3</v>
       </c>
-      <c r="K3" s="10">
+      <c r="J3" s="10">
         <f t="shared" si="0"/>
         <v>0.21666666666666723</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17">
+    <row r="4" spans="1:10" ht="17">
       <c r="A4" s="6">
         <f>IF(B4&lt;&gt;"",A3,"")</f>
         <v>43102</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="7" t="s">
-        <v>8</v>
+      <c r="G4" s="9">
+        <v>0.3215277777777778</v>
       </c>
       <c r="H4" s="9">
-        <v>0.3215277777777778</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="I4" s="9">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="J4" s="9">
-        <f>IF(AND(H4&lt;&gt;"",I4&lt;&gt;""),I4-H4,"")</f>
+        <f>IF(AND(G4&lt;&gt;"",H4&lt;&gt;""),H4-G4,"")</f>
         <v>3.2638888888888884E-2</v>
       </c>
-      <c r="K4" s="10">
+      <c r="J4" s="10">
         <f t="shared" si="0"/>
         <v>0.78333333333333321</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17">
+    <row r="5" spans="1:10" ht="17">
       <c r="A5" s="6">
         <v>43103</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="7" t="s">
-        <v>10</v>
+      <c r="G5" s="9">
+        <v>0.35416666666666669</v>
       </c>
       <c r="H5" s="9">
-        <v>0.35416666666666669</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="I5" s="9">
-        <v>0.40972222222222227</v>
-      </c>
-      <c r="J5" s="9">
-        <f>IF(AND(H5&lt;&gt;"",I5&lt;&gt;""),I5-H5,"")</f>
+        <f>IF(AND(G5&lt;&gt;"",H5&lt;&gt;""),H5-G5,"")</f>
         <v>5.555555555555558E-2</v>
       </c>
-      <c r="K5" s="10">
+      <c r="J5" s="10">
         <f t="shared" si="0"/>
         <v>1.3333333333333339</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17">
+    <row r="6" spans="1:10" ht="17">
       <c r="A6" s="6">
         <v>43104</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="7" t="s">
-        <v>34</v>
+      <c r="F6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.49305555555555558</v>
       </c>
       <c r="H6" s="9">
-        <v>0.49305555555555558</v>
+        <v>0.59375</v>
       </c>
       <c r="I6" s="9">
-        <v>0.59375</v>
-      </c>
-      <c r="J6" s="9">
-        <f>IF(AND(H6&lt;&gt;"",I6&lt;&gt;""),I6-H6,"")</f>
+        <f>IF(AND(G6&lt;&gt;"",H6&lt;&gt;""),H6-G6,"")</f>
         <v>0.10069444444444442</v>
       </c>
-      <c r="K6" s="10">
+      <c r="J6" s="10">
         <f t="shared" si="0"/>
         <v>2.4166666666666661</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17">
+    <row r="7" spans="1:10" ht="17">
       <c r="A7" s="6">
         <v>43105</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="F7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9">
+      <c r="I7" s="9">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="K7" s="10">
+      <c r="J7" s="10">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17">
+    <row r="8" spans="1:10" ht="17">
       <c r="A8" s="6">
         <v>43108</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="F8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9">
+      <c r="I8" s="9">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="K8" s="10">
+      <c r="J8" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="17">
+    <row r="9" spans="1:10" ht="17">
       <c r="A9" s="6">
         <v>43109</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="7" t="s">
-        <v>13</v>
+      <c r="F9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="9">
+        <v>5.2083333333333336E-2</v>
       </c>
       <c r="H9" s="9">
-        <v>5.2083333333333336E-2</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="I9" s="9">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="J9" s="9">
-        <f t="shared" ref="J9:J15" si="1">IF(AND(H9&lt;&gt;"",I9&lt;&gt;""),I9-H9,"")</f>
+        <f t="shared" ref="I9:I15" si="1">IF(AND(G9&lt;&gt;"",H9&lt;&gt;""),H9-G9,"")</f>
         <v>9.375E-2</v>
       </c>
-      <c r="K9" s="10">
+      <c r="J9" s="10">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17">
+    <row r="10" spans="1:10" ht="17">
       <c r="A10" s="6">
         <f>IF(B10&lt;&gt;"",A9,"")</f>
         <v>43109</v>
@@ -956,165 +939,158 @@
         <v>Customer 2</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7" t="s">
-        <v>13</v>
+      <c r="F10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0.2638888888888889</v>
       </c>
       <c r="H10" s="9">
-        <v>0.2638888888888889</v>
+        <v>0.28472222222222221</v>
       </c>
       <c r="I10" s="9">
-        <v>0.28472222222222221</v>
-      </c>
-      <c r="J10" s="9">
         <f t="shared" si="1"/>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="K10" s="10">
+      <c r="J10" s="10">
         <f t="shared" si="0"/>
         <v>0.49999999999999956</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17">
+    <row r="11" spans="1:10" ht="17">
       <c r="A11" s="6">
         <v>43110</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="7" t="s">
-        <v>14</v>
+      <c r="F11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0.47916666666666669</v>
       </c>
       <c r="H11" s="9">
-        <v>0.47916666666666669</v>
+        <v>0.5</v>
       </c>
       <c r="I11" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="J11" s="9">
         <f t="shared" si="1"/>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="K11" s="10">
+      <c r="J11" s="10">
         <f t="shared" si="0"/>
         <v>0.49999999999999956</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17">
+    <row r="12" spans="1:10" ht="17">
       <c r="A12" s="6">
         <v>43111</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="7" t="s">
-        <v>15</v>
+      <c r="F12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.21875</v>
       </c>
       <c r="H12" s="9">
-        <v>0.21875</v>
+        <v>0.23958333333333334</v>
       </c>
       <c r="I12" s="9">
-        <v>0.23958333333333334</v>
-      </c>
-      <c r="J12" s="9">
         <f t="shared" si="1"/>
         <v>2.0833333333333343E-2</v>
       </c>
-      <c r="K12" s="10">
+      <c r="J12" s="10">
         <f t="shared" si="0"/>
         <v>0.50000000000000022</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17">
+    <row r="13" spans="1:10" ht="17">
       <c r="A13" s="6">
         <f>IF(B13&lt;&gt;"",A12,"")</f>
         <v>43111</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="7" t="s">
-        <v>16</v>
+      <c r="F13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.25</v>
       </c>
       <c r="H13" s="9">
-        <v>0.25</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="I13" s="9">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="J13" s="9">
         <f t="shared" si="1"/>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="K13" s="10">
+      <c r="J13" s="10">
         <f t="shared" si="0"/>
         <v>0.49999999999999956</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17">
+    <row r="14" spans="1:10" ht="17">
       <c r="A14" s="6">
         <v>43111</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>36</v>
+      <c r="F14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0.3298611111111111</v>
       </c>
       <c r="H14" s="9">
-        <v>0.3298611111111111</v>
+        <v>0.3576388888888889</v>
       </c>
       <c r="I14" s="9">
-        <v>0.3576388888888889</v>
-      </c>
-      <c r="J14" s="9">
         <f t="shared" si="1"/>
         <v>2.777777777777779E-2</v>
       </c>
-      <c r="K14" s="10">
+      <c r="J14" s="10">
         <f t="shared" si="0"/>
         <v>0.66666666666666696</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="17">
+    <row r="15" spans="1:10" ht="17">
       <c r="A15" s="6">
         <f>IF(B15&lt;&gt;"",A14,"")</f>
         <v>43111</v>
@@ -1124,32 +1100,31 @@
         <v>Customer 3</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="7" t="s">
-        <v>17</v>
+      <c r="F15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.33333333333333331</v>
       </c>
       <c r="H15" s="9">
-        <v>0.33333333333333331</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="I15" s="9">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="J15" s="9">
         <f t="shared" si="1"/>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="K15" s="10">
+      <c r="J15" s="10">
         <f t="shared" si="0"/>
         <v>0.50000000000000089</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17">
+    <row r="16" spans="1:10" ht="17">
       <c r="A16" s="6">
         <f>IF(B16&lt;&gt;"",A15,"")</f>
         <v>43111</v>
@@ -1159,160 +1134,151 @@
         <v>Customer 3</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="F16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="9"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9">
+      <c r="I16" s="9">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="K16" s="10">
+      <c r="J16" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="17">
+    <row r="17" spans="1:10" ht="17">
       <c r="A17" s="6">
         <v>43112</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>38</v>
+      <c r="F17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0.48958333333333331</v>
       </c>
       <c r="H17" s="9">
-        <v>0.48958333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="I17" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="J17" s="9">
-        <f t="shared" ref="J17:J27" si="2">IF(AND(H17&lt;&gt;"",I17&lt;&gt;""),I17-H17,"")</f>
+        <f t="shared" ref="I17:I27" si="2">IF(AND(G17&lt;&gt;"",H17&lt;&gt;""),H17-G17,"")</f>
         <v>1.0416666666666685E-2</v>
       </c>
-      <c r="K17" s="10">
+      <c r="J17" s="10">
         <f t="shared" si="0"/>
         <v>0.25000000000000044</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="17">
+    <row r="18" spans="1:10" ht="17">
       <c r="A18" s="6">
         <v>43115</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="7" t="s">
-        <v>18</v>
+      <c r="F18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0.11458333333333333</v>
       </c>
       <c r="H18" s="9">
-        <v>0.11458333333333333</v>
+        <v>0.18055555555555555</v>
       </c>
       <c r="I18" s="9">
-        <v>0.18055555555555555</v>
-      </c>
-      <c r="J18" s="9">
         <f t="shared" si="2"/>
         <v>6.5972222222222224E-2</v>
       </c>
-      <c r="K18" s="10">
+      <c r="J18" s="10">
         <f t="shared" si="0"/>
         <v>1.5833333333333335</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17">
+    <row r="19" spans="1:10" ht="17">
       <c r="A19" s="6">
         <v>43117</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="7" t="s">
-        <v>19</v>
+      <c r="F19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0.54166666666666663</v>
       </c>
       <c r="H19" s="9">
-        <v>0.54166666666666663</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="I19" s="9">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="J19" s="9">
         <f t="shared" si="2"/>
         <v>1.3888888888888951E-2</v>
       </c>
-      <c r="K19" s="10">
+      <c r="J19" s="10">
         <f t="shared" si="0"/>
         <v>0.33333333333333481</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="17">
+    <row r="20" spans="1:10" ht="17">
       <c r="A20" s="6">
         <f>IF(B20&lt;&gt;"",A19,"")</f>
         <v>43117</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="7" t="s">
-        <v>20</v>
+      <c r="F20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0.5625</v>
       </c>
       <c r="H20" s="9">
-        <v>0.5625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I20" s="9">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="J20" s="9">
         <f t="shared" si="2"/>
         <v>0.10416666666666663</v>
       </c>
-      <c r="K20" s="10">
+      <c r="J20" s="10">
         <f t="shared" si="0"/>
         <v>2.4999999999999991</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="17">
+    <row r="21" spans="1:10" ht="17">
       <c r="A21" s="6">
         <f>IF(B21&lt;&gt;"",A20,"")</f>
         <v>43117</v>
@@ -1322,166 +1288,161 @@
         <v>Customer 4</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="7" t="s">
-        <v>19</v>
+      <c r="F21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0.58333333333333337</v>
       </c>
       <c r="H21" s="9">
-        <v>0.58333333333333337</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I21" s="9">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="J21" s="9">
         <f t="shared" si="2"/>
         <v>6.25E-2</v>
       </c>
-      <c r="K21" s="10">
+      <c r="J21" s="10">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="17">
+    <row r="22" spans="1:10" ht="17">
       <c r="A22" s="6">
         <f>IF(B22&lt;&gt;"",A21,"")</f>
         <v>43117</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="7" t="s">
-        <v>19</v>
+      <c r="F22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0.8125</v>
       </c>
       <c r="H22" s="9">
-        <v>0.8125</v>
+        <v>0.84375</v>
       </c>
       <c r="I22" s="9">
-        <v>0.84375</v>
-      </c>
-      <c r="J22" s="9">
         <f t="shared" si="2"/>
         <v>3.125E-2</v>
       </c>
-      <c r="K22" s="10">
+      <c r="J22" s="10">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17">
+    <row r="23" spans="1:10" ht="17">
       <c r="A23" s="6">
         <v>43117</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="7" t="s">
-        <v>22</v>
+      <c r="G23" s="9">
+        <v>0.82986111111111116</v>
       </c>
       <c r="H23" s="9">
-        <v>0.82986111111111116</v>
+        <v>0.87152777777777779</v>
       </c>
       <c r="I23" s="9">
-        <v>0.87152777777777779</v>
-      </c>
-      <c r="J23" s="9">
         <f t="shared" si="2"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="K23" s="10">
+      <c r="J23" s="10">
         <f t="shared" si="0"/>
         <v>0.99999999999999911</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="17">
+    <row r="24" spans="1:10" ht="17">
       <c r="A24" s="6">
         <f>IF(B24&lt;&gt;"",A23,"")</f>
         <v>43117</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="7" t="s">
-        <v>39</v>
+      <c r="F24" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0.875</v>
       </c>
       <c r="H24" s="9">
-        <v>0.875</v>
+        <v>0.92708333333333337</v>
       </c>
       <c r="I24" s="9">
-        <v>0.92708333333333337</v>
-      </c>
-      <c r="J24" s="9">
         <f t="shared" si="2"/>
         <v>5.208333333333337E-2</v>
       </c>
-      <c r="K24" s="10">
+      <c r="J24" s="10">
         <f t="shared" si="0"/>
         <v>1.2500000000000009</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="17">
+    <row r="25" spans="1:10" ht="17">
       <c r="A25" s="6">
         <v>43118</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="7" t="s">
-        <v>40</v>
+      <c r="F25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="9">
+        <v>9.0277777777777776E-2</v>
       </c>
       <c r="H25" s="9">
-        <v>9.0277777777777776E-2</v>
+        <v>0.15277777777777776</v>
       </c>
       <c r="I25" s="9">
-        <v>0.15277777777777776</v>
-      </c>
-      <c r="J25" s="9">
         <f t="shared" si="2"/>
         <v>6.2499999999999986E-2</v>
       </c>
-      <c r="K25" s="10">
+      <c r="J25" s="10">
         <f t="shared" si="0"/>
         <v>1.4999999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="17">
+    <row r="26" spans="1:10" ht="17">
       <c r="A26" s="6">
         <f>IF(B26&lt;&gt;"",A25,"")</f>
         <v>43118</v>
@@ -1491,32 +1452,31 @@
         <v>Customer 1</v>
       </c>
       <c r="C26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="7" t="s">
-        <v>24</v>
+      <c r="G26" s="9">
+        <v>0.3611111111111111</v>
       </c>
       <c r="H26" s="9">
-        <v>0.3611111111111111</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="I26" s="9">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="J26" s="9">
         <f t="shared" si="2"/>
         <v>5.555555555555558E-2</v>
       </c>
-      <c r="K26" s="10">
+      <c r="J26" s="10">
         <f t="shared" si="0"/>
         <v>1.3333333333333339</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="17">
+    <row r="27" spans="1:10" ht="17">
       <c r="A27" s="6">
         <f>IF(B27&lt;&gt;"",A26,"")</f>
         <v>43118</v>
@@ -1526,27 +1486,26 @@
         <v>Customer 1</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="7" t="s">
-        <v>41</v>
+      <c r="F27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0.73263888888888884</v>
       </c>
       <c r="H27" s="9">
-        <v>0.73263888888888884</v>
+        <v>0.74305555555555547</v>
       </c>
       <c r="I27" s="9">
-        <v>0.74305555555555547</v>
-      </c>
-      <c r="J27" s="9">
         <f t="shared" si="2"/>
         <v>1.041666666666663E-2</v>
       </c>
-      <c r="K27" s="10">
+      <c r="J27" s="10">
         <f t="shared" si="0"/>
         <v>0.24999999999999911</v>
       </c>

</xml_diff>